<commit_message>
MAINT: Before running script
</commit_message>
<xml_diff>
--- a/MISO/Constraint Analyses/Top Congestion Reports/Oct-24_RT.xlsx
+++ b/MISO/Constraint Analyses/Top Congestion Reports/Oct-24_RT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://roscommonanalytics-my.sharepoint.com/personal/lgraham_roscommonanalytics_com/Documents/Documents/Obsidian_Vault/MISO/Constraint Analyses/Top Congestion Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="8_{2362F2EE-3FDA-45C7-8C6F-19B413AE0C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42CB5163-E244-4274-A482-1B495D2B6277}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{2362F2EE-3FDA-45C7-8C6F-19B413AE0C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F781BEF-6D21-4C08-A71A-7885995E12AA}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{49B1CF11-8F84-48E4-A133-6DB4C44CF737}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="109">
   <si>
     <t>cid</t>
   </si>
@@ -351,13 +351,19 @@
     <t>Ft. Thompson-Oahe Dam Ckt 2 230 kV outage (case outage -- no corresponding ticket!). Excess MDU load. Week MDU wind generation. Summer ratings.</t>
   </si>
   <si>
-    <t>Summer ratings. Uprates Nov. 1</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
     <t>Winter ratings from 11/1-4/1. Winter (only) B-ratings uprated from 131 MW to 169 MW in Winter 2024-25.</t>
+  </si>
+  <si>
+    <t>Summer ratings. Eastward wind transfer from MISO into SPP. Lisbon-Enderlin 69 kV outage.</t>
+  </si>
+  <si>
+    <t>Southward wind transfer from the greater Sioux City, IA area (including SPP) into Omaha, NE. Flows show a strong negative correlation with Walter Scott Jr. output.</t>
+  </si>
+  <si>
+    <t>Curious B-rating uprate on 11/8/2024 from 217 MW to 284 MW. This was followed by a 1/30/2025 B-rating derate from 284 MW to 259 MW then again on 2/21/2025 from 259 MW to 256 MW and again on 4/7/2025 from 256 MW to 217 MW. Tekamah-Oakland 115 kV is a switching solution that relieves Tekamah-Substation 1226 at the expense of increasing flows on Raun-Tekamah.</t>
   </si>
 </sst>
 </file>
@@ -762,7 +768,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,7 +836,7 @@
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -924,10 +930,10 @@
         <v>28</v>
       </c>
       <c r="O3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="P3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -972,6 +978,12 @@
       </c>
       <c r="N4" t="s">
         <v>31</v>
+      </c>
+      <c r="O4" t="s">
+        <v>107</v>
+      </c>
+      <c r="P4" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1729,10 +1741,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72FE7B81-3610-4931-AC6B-486B63B77EEA}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4:P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1753,7 +1765,7 @@
     <col min="15" max="15" width="117.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1799,8 +1811,11 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>314718</v>
       </c>
@@ -1843,8 +1858,14 @@
       <c r="N2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>106</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>396264</v>
       </c>
@@ -1888,7 +1909,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>77127</v>
       </c>
@@ -1931,8 +1952,14 @@
       <c r="N4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O4" t="s">
+        <v>107</v>
+      </c>
+      <c r="P4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>455851</v>
       </c>
@@ -1976,7 +2003,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>306800</v>
       </c>
@@ -2020,7 +2047,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>350280</v>
       </c>
@@ -2067,7 +2094,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>465036</v>
       </c>
@@ -2111,7 +2138,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>375350</v>
       </c>
@@ -2155,7 +2182,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>344916</v>
       </c>
@@ -2199,7 +2226,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>72687</v>
       </c>
@@ -2243,7 +2270,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>333296</v>
       </c>
@@ -2287,7 +2314,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>462022</v>
       </c>
@@ -2331,7 +2358,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>349600</v>
       </c>
@@ -2375,7 +2402,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>349896</v>
       </c>
@@ -2419,7 +2446,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>463281</v>
       </c>

</xml_diff>

<commit_message>
ENH: Add Oct-24 notes
</commit_message>
<xml_diff>
--- a/MISO/Constraint Analyses/Top Congestion Reports/Oct-24_RT.xlsx
+++ b/MISO/Constraint Analyses/Top Congestion Reports/Oct-24_RT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://roscommonanalytics-my.sharepoint.com/personal/lgraham_roscommonanalytics_com/Documents/Documents/Obsidian_Vault/MISO/Constraint Analyses/Top Congestion Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="8_{2362F2EE-3FDA-45C7-8C6F-19B413AE0C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F781BEF-6D21-4C08-A71A-7885995E12AA}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="8_{2362F2EE-3FDA-45C7-8C6F-19B413AE0C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0469C68-C647-4FEC-B73E-D98E3D50A4FC}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{49B1CF11-8F84-48E4-A133-6DB4C44CF737}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="138">
   <si>
     <t>cid</t>
   </si>
@@ -364,6 +364,93 @@
   </si>
   <si>
     <t>Curious B-rating uprate on 11/8/2024 from 217 MW to 284 MW. This was followed by a 1/30/2025 B-rating derate from 284 MW to 259 MW then again on 2/21/2025 from 259 MW to 256 MW and again on 4/7/2025 from 256 MW to 217 MW. Tekamah-Oakland 115 kV is a switching solution that relieves Tekamah-Substation 1226 at the expense of increasing flows on Raun-Tekamah.</t>
+  </si>
+  <si>
+    <t>Severe, unprecedented derate. Clean relationship between binding events and the derate. Hasn't bound since.</t>
+  </si>
+  <si>
+    <t>Mt. Vernon-W. Frankfort 230 kV outage. Moderate sum of wind generation and coal generation. Load to the South, Southeast.</t>
+  </si>
+  <si>
+    <t>Bound often before 12/17/2024. A clear regime change occurred on 12/18/2024 which drastically reduced post-contingent flow.</t>
+  </si>
+  <si>
+    <t>Diamond Trail-Hills 345 kV, Powesheik Co-Reasnor 161 kV outages. Wind push.</t>
+  </si>
+  <si>
+    <t>Big Stone TR 230/115 kV, Benson-Swenoda 115 kV outages increased binding likelihood.</t>
+  </si>
+  <si>
+    <t>Weak wind in OTP and high Boswell generation.</t>
+  </si>
+  <si>
+    <t>Doud-Boone Junction 161 kV, Karma-Perry 161 kV outages. Story County, Great Pathfinder wind generation.</t>
+  </si>
+  <si>
+    <t>Sarepta-Longwood 345 kV outage. Weak Harrison County generation. Weak OK wind generation.</t>
+  </si>
+  <si>
+    <t>Thomas Hill-Mead 161 kV outage. Heavy SPP wind generation. Thomas Hill outage.</t>
+  </si>
+  <si>
+    <t>White Cloud, Clear Creek, Rock Creek wind generation. Southwest IA wind generation. Excess load in St. Joseph, Kansas City.</t>
+  </si>
+  <si>
+    <t>Excess ComEd generation. Excess MEC generation. Sheffield-Gary Ave-Dune Acres 345 kV outages. Chicago Ave-Gary Ave 138 kV outage.</t>
+  </si>
+  <si>
+    <t>Southward wind transfer from IA into MO. Hills-Diamond Trails 345 kV outage.</t>
+  </si>
+  <si>
+    <t>Reasnor-Poweshiek Co-Irvine 161 kV outages. Hills-Diamond Trail 345 kV outage. Knoxville-Lucas 69 kV outages. Grinnell-S. Grinnell 69 kV outage.</t>
+  </si>
+  <si>
+    <t>Southward wind transfer from IA into MO. Hills-Diamond Trails 345 kV outage. High wind generation. Low Ottumwa output.</t>
+  </si>
+  <si>
+    <t>Eastward wind transfer from South Central IA to Southeast IA and IL. Hills-Diamond Trail 345 kV outage.  High wind generation. Excess MEC, ALTW generation.</t>
+  </si>
+  <si>
+    <t>Clear relationship with Hazleton-Arnold 345 kV outage, which bottlenecks wind supply from IA and forces it over the constraint.</t>
+  </si>
+  <si>
+    <t>Floyd-Emery-Sheffield, Worth Co-Glenville-Hayward 161 kV outages. Wind generation in Northern IA.</t>
+  </si>
+  <si>
+    <t>Cordova-Substation 39 345 kV outage. Quad Cities push.</t>
+  </si>
+  <si>
+    <t>Big Stone TR 230/115 kV, Big Stone-Brownsville 230 kV outages. High sensitivity to wind push at Dakota Range, Crowned Ridge, Deuel Harvest, etc. Clean relationship with Big Stone TR outage.</t>
+  </si>
+  <si>
+    <t>Harmony-Lansing 161 kV outage.</t>
+  </si>
+  <si>
+    <t>This is odd, as it looks like the monitored element is radial. I'm not fully sure what's going on here.</t>
+  </si>
+  <si>
+    <t>Sarepta-Longwood 345 kV outage. ERCOT East DC tie line "load."</t>
+  </si>
+  <si>
+    <t>Bound briefly before substantial uprate on 10/29/2025 from 198 MW to 357 MW (post-contingent). Unlikely to bind in the current regime.</t>
+  </si>
+  <si>
+    <t>Monticello-Lafayette-Lafayette LC 138 kV outages.</t>
+  </si>
+  <si>
+    <t>Winger-Riverton, Hubbard-Audubon 230 kV outages. Wind generation to the West.</t>
+  </si>
+  <si>
+    <t>Maryville-Maryville 161 kV outage (extreme impact). Highly sensitive to Clear Creek, White Cloud wind push in the post-contingent setting with Maryville-Maryville 161 kV OOS.</t>
+  </si>
+  <si>
+    <t>Palisades-Argenta-Tompkins, Battle Ck-Oneida 345 kV outages. Verona-Convis 138 kV outage.</t>
+  </si>
+  <si>
+    <t>Will not bind when Calhoun Solar, Cereal City Solar are generating.</t>
+  </si>
+  <si>
+    <t>Wind transfer stepping down to 115 kV level. Clean relationship with Chub Lk-Hampton 345 kV outage. Excess MEC supply.</t>
   </si>
 </sst>
 </file>
@@ -767,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD27041E-A0E1-4723-A2AA-E563763CB453}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,6 +1116,9 @@
       <c r="N5" t="s">
         <v>34</v>
       </c>
+      <c r="O5" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -1073,6 +1163,9 @@
       <c r="N6" t="s">
         <v>37</v>
       </c>
+      <c r="O6" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -1117,6 +1210,9 @@
       <c r="N7" t="s">
         <v>40</v>
       </c>
+      <c r="O7" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -1161,6 +1257,9 @@
       <c r="N8" t="s">
         <v>43</v>
       </c>
+      <c r="O8" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -1205,6 +1304,9 @@
       <c r="N9" t="s">
         <v>46</v>
       </c>
+      <c r="O9" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -1249,6 +1351,9 @@
       <c r="N10" t="s">
         <v>49</v>
       </c>
+      <c r="O10" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -1293,6 +1398,9 @@
       <c r="N11" t="s">
         <v>52</v>
       </c>
+      <c r="O11" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -1337,6 +1445,9 @@
       <c r="N12" t="s">
         <v>55</v>
       </c>
+      <c r="O12" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -1381,6 +1492,9 @@
       <c r="N13" t="s">
         <v>58</v>
       </c>
+      <c r="O13" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -1425,6 +1539,9 @@
       <c r="N14" t="s">
         <v>60</v>
       </c>
+      <c r="O14" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -1469,6 +1586,12 @@
       <c r="N15" t="s">
         <v>63</v>
       </c>
+      <c r="O15" t="s">
+        <v>132</v>
+      </c>
+      <c r="P15" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -1513,8 +1636,11 @@
       <c r="N16" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>465036</v>
       </c>
@@ -1557,8 +1683,11 @@
       <c r="N17" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>62613</v>
       </c>
@@ -1601,8 +1730,14 @@
       <c r="N18" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18" t="s">
+        <v>128</v>
+      </c>
+      <c r="P18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>324540</v>
       </c>
@@ -1645,8 +1780,11 @@
       <c r="N19" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>349600</v>
       </c>
@@ -1689,8 +1827,11 @@
       <c r="N20" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>344566</v>
       </c>
@@ -1732,6 +1873,9 @@
       </c>
       <c r="N21" t="s">
         <v>80</v>
+      </c>
+      <c r="O21" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1744,7 +1888,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4:P4"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1908,6 +2052,9 @@
       <c r="N3" t="s">
         <v>37</v>
       </c>
+      <c r="O3" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -2002,6 +2149,9 @@
       <c r="N5" t="s">
         <v>34</v>
       </c>
+      <c r="O5" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -2046,6 +2196,9 @@
       <c r="N6" t="s">
         <v>43</v>
       </c>
+      <c r="O6" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -2137,6 +2290,9 @@
       <c r="N8" t="s">
         <v>68</v>
       </c>
+      <c r="O8" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -2181,6 +2337,9 @@
       <c r="N9" t="s">
         <v>84</v>
       </c>
+      <c r="O9" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -2225,6 +2384,9 @@
       <c r="N10" t="s">
         <v>19</v>
       </c>
+      <c r="O10" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -2269,6 +2431,9 @@
       <c r="N11" t="s">
         <v>22</v>
       </c>
+      <c r="O11" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -2313,6 +2478,9 @@
       <c r="N12" t="s">
         <v>77</v>
       </c>
+      <c r="O12" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -2357,6 +2525,9 @@
       <c r="N13" t="s">
         <v>87</v>
       </c>
+      <c r="O13" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -2401,6 +2572,9 @@
       <c r="N14" t="s">
         <v>77</v>
       </c>
+      <c r="O14" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -2445,6 +2619,9 @@
       <c r="N15" t="s">
         <v>55</v>
       </c>
+      <c r="O15" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -2489,8 +2666,11 @@
       <c r="N16" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>344566</v>
       </c>
@@ -2533,8 +2713,11 @@
       <c r="N17" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>302332</v>
       </c>
@@ -2577,8 +2760,11 @@
       <c r="N18" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>347564</v>
       </c>
@@ -2621,8 +2807,11 @@
       <c r="N19" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>416410</v>
       </c>
@@ -2665,8 +2854,14 @@
       <c r="N20" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20" t="s">
+        <v>135</v>
+      </c>
+      <c r="P20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>360096</v>
       </c>
@@ -2708,6 +2903,9 @@
       </c>
       <c r="N21" t="s">
         <v>102</v>
+      </c>
+      <c r="O21" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>